<commit_message>
Detected Bug B3 in TC10.2
</commit_message>
<xml_diff>
--- a/Requirements/Testing/10-Modify Label.xlsx
+++ b/Requirements/Testing/10-Modify Label.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caeta\Desktop\Documents\Proyectos\TimeAdministrator\TimeAdministrator\Requirements\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596C0F7C-4867-4CFA-BFCF-EE585E04B422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7109F44-1C64-4626-A31E-4D3BF34D17D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20910" windowHeight="13740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20910" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC10.1" sheetId="1" r:id="rId1"/>
@@ -346,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -362,9 +362,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -387,9 +384,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -404,6 +398,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -695,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,285 +765,285 @@
       <c r="B2" s="7">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="15" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="11" t="s">
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="14"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="24"/>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="15" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11" t="s">
+      <c r="H4" s="13"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="17"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="15" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="18" t="s">
+      <c r="H5" s="13"/>
+      <c r="I5" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="17"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="16"/>
     </row>
     <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="14" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="15" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="17"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="15" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="17"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="16"/>
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="15" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="17"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="16"/>
     </row>
     <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="15" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="17"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="16"/>
     </row>
     <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="15" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="17"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="16"/>
     </row>
     <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="15" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="17"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="16"/>
     </row>
     <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="15" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="17"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="16"/>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="17"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="16"/>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="17"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="17"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="16"/>
     </row>
     <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="17"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="16"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -1051,21 +1054,21 @@
       <c r="U16" s="3"/>
     </row>
     <row r="17" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="22"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="20"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
@@ -1083,9 +1086,9 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="E2:E4"/>
-    <mergeCell ref="H2:H16"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="I5:I7"/>
+    <mergeCell ref="H2:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1095,7 +1098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0184EBC7-3D9A-4071-9A07-2A893239CD8F}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2:M5"/>
     </sheetView>
   </sheetViews>
@@ -1163,306 +1166,306 @@
       <c r="B2" s="7">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="23" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="15" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="11" t="s">
+      <c r="H3" s="24"/>
+      <c r="I3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11" t="s">
+      <c r="J3" s="10"/>
+      <c r="K3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="14"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="24"/>
     </row>
     <row r="4" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="15" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="14"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="24"/>
     </row>
     <row r="5" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="15" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14" t="s">
+      <c r="H5" s="24"/>
+      <c r="I5" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="14"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="24"/>
     </row>
     <row r="6" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="14" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="15" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="11"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="10"/>
     </row>
     <row r="7" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="15" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="17"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="16"/>
     </row>
     <row r="8" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="15" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="17"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="16"/>
     </row>
     <row r="9" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="15" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="17"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="16"/>
     </row>
     <row r="10" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="15" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="17"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="16"/>
     </row>
     <row r="11" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="15" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="17"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="16"/>
     </row>
     <row r="12" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="15" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="17"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="16"/>
     </row>
     <row r="13" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="17"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="16"/>
     </row>
     <row r="14" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="17"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="17"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="16"/>
     </row>
     <row r="16" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="17"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="16"/>
     </row>
     <row r="17" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="23" t="s">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="22"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>